<commit_message>
Modal crear nueva caja, pasos de crear caja
</commit_message>
<xml_diff>
--- a/Material de apoyo/Recursos.xlsx
+++ b/Material de apoyo/Recursos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARCHIVOS\INACAP\SEPTIMO SEMESTRE\TALLER DE PROYECTO DE SOFTWARE\UNIDAD 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\TIDC24-EQUIPO-4\Material de apoyo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA117D98-2860-463C-B9B4-1C732E31B989}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2D3F5C-FAE8-467D-BB07-20D2EDC3667F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E570FF1-879C-4355-B744-693133030B04}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6E570FF1-879C-4355-B744-693133030B04}"/>
   </bookViews>
   <sheets>
     <sheet name="Gastos materiales" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,6 +450,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -490,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -502,11 +508,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -830,7 +839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3661391-4A29-49C5-9CAC-9BFB4A276F1A}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
@@ -1113,7 +1122,7 @@
       <c r="B6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="7" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1124,7 +1133,7 @@
       <c r="B7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -1133,7 +1142,7 @@
       <c r="B8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -1142,7 +1151,7 @@
       <c r="B9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -1151,7 +1160,7 @@
       <c r="B10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -1160,7 +1169,7 @@
       <c r="B11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -1169,7 +1178,7 @@
       <c r="B12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -1178,7 +1187,7 @@
       <c r="B13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -1187,7 +1196,7 @@
       <c r="B14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -1196,7 +1205,7 @@
       <c r="B15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -1205,7 +1214,7 @@
       <c r="B16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -1214,7 +1223,7 @@
       <c r="B17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="7"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -1223,7 +1232,7 @@
       <c r="B18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="5"/>
+      <c r="C18" s="7"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -1232,7 +1241,7 @@
       <c r="B19" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="7"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -1241,7 +1250,7 @@
       <c r="B20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="5"/>
+      <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -1250,7 +1259,7 @@
       <c r="B21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="7"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
@@ -1259,7 +1268,7 @@
       <c r="B22" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="5"/>
+      <c r="C22" s="7"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -1268,7 +1277,7 @@
       <c r="B23" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -1277,7 +1286,7 @@
       <c r="B24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="5"/>
+      <c r="C24" s="7"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
@@ -1286,7 +1295,7 @@
       <c r="B25" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="5"/>
+      <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
@@ -1295,7 +1304,7 @@
       <c r="B26" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="5"/>
+      <c r="C26" s="7"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
@@ -1304,7 +1313,7 @@
       <c r="B27" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
@@ -1313,7 +1322,7 @@
       <c r="B28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="5"/>
+      <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -1322,7 +1331,7 @@
       <c r="B29" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="5"/>
+      <c r="C29" s="7"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
@@ -1331,7 +1340,7 @@
       <c r="B30" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="5"/>
+      <c r="C30" s="7"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
@@ -1340,7 +1349,7 @@
       <c r="B31" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="5"/>
+      <c r="C31" s="7"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
@@ -1349,7 +1358,7 @@
       <c r="B32" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="5"/>
+      <c r="C32" s="7"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
@@ -1358,7 +1367,7 @@
       <c r="B33" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="5"/>
+      <c r="C33" s="7"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
@@ -1367,7 +1376,7 @@
       <c r="B34" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="5"/>
+      <c r="C34" s="7"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
@@ -1376,7 +1385,7 @@
       <c r="B35" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="5"/>
+      <c r="C35" s="7"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
@@ -1385,7 +1394,7 @@
       <c r="B36" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="5"/>
+      <c r="C36" s="7"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
@@ -1394,7 +1403,7 @@
       <c r="B37" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="5"/>
+      <c r="C37" s="7"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
@@ -1403,7 +1412,7 @@
       <c r="B38" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="5"/>
+      <c r="C38" s="7"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
@@ -1412,7 +1421,7 @@
       <c r="B39" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C39" s="5"/>
+      <c r="C39" s="7"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
@@ -1421,7 +1430,7 @@
       <c r="B40" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="5"/>
+      <c r="C40" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1669,8 +1678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9304C130-7E3F-4524-8988-0073E55933CF}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1681,18 +1690,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>109</v>
       </c>
       <c r="C2" t="s">
@@ -1700,18 +1709,18 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>111</v>
       </c>
       <c r="C4" t="s">
@@ -1719,18 +1728,18 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>115</v>
       </c>
       <c r="C6" t="s">
@@ -1738,18 +1747,18 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1773,66 +1782,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>